<commit_message>
Fixed import of cashflows
</commit_message>
<xml_diff>
--- a/public/sample_uploads/portfolio_income.xlsx
+++ b/public/sample_uploads/portfolio_income.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aseem Karmali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDD8AC5-DF10-41B3-93F3-15726F07BFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEF1515-EC96-4DFB-BA9D-A4FE9A1FB399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -207,7 +207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{D8613426-BD5A-43E6-85EB-2B1AD0F043C1}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{03264531-5020-4873-AAF0-E9ABB422599F}">
       <text>
         <r>
           <rPr>
@@ -215,7 +215,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -224,15 +224,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
--Mandatory
--As per SEBI reporting requirements</t>
+-Optional</t>
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{29805756-4084-4236-A5D7-9799CFA6F357}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00025E97-2F1E-4D72-9753-8CF0D32D3DCA}">
       <text>
         <r>
           <rPr>
@@ -240,7 +239,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -249,36 +248,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
--Mandatory
--As per SEBI reporting requirements</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{1F43627D-F125-4CD3-96EA-01A92B934F8D}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
--Mandatory
--As per SEBI reporting requirements</t>
+-Mandatory</t>
         </r>
       </text>
     </comment>
@@ -287,7 +260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>Amount *</t>
   </si>
@@ -298,15 +271,6 @@
     <t>Folio No</t>
   </si>
   <si>
-    <t>Category *</t>
-  </si>
-  <si>
-    <t>Sub Category *</t>
-  </si>
-  <si>
-    <t>Investment Domicile *</t>
-  </si>
-  <si>
     <t>SAAS Fund</t>
   </si>
   <si>
@@ -316,15 +280,6 @@
     <t>Pool</t>
   </si>
   <si>
-    <t>Unlisted</t>
-  </si>
-  <si>
-    <t>Equity</t>
-  </si>
-  <si>
-    <t>Domestic</t>
-  </si>
-  <si>
     <t>CoInvest</t>
   </si>
   <si>
@@ -358,14 +313,14 @@
     <t>Tag</t>
   </si>
   <si>
-    <t>Instrument</t>
+    <t>Instrument *</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -414,6 +369,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -769,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -780,27 +748,26 @@
     <col min="1" max="1" width="10.19921875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.73046875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.19921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.06640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.9296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.19921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.9296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.19921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="1015" width="8.53125" style="2"/>
-    <col min="1016" max="1016" width="9.1328125" style="2" customWidth="1"/>
-    <col min="1017" max="16384" width="8.53125" style="2"/>
+    <col min="6" max="6" width="10" style="4" customWidth="1"/>
+    <col min="7" max="7" width="9.59765625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="6.9296875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.9296875" style="2" customWidth="1"/>
+    <col min="10" max="1012" width="8.53125" style="2"/>
+    <col min="1013" max="1013" width="9.1328125" style="2" customWidth="1"/>
+    <col min="1014" max="16384" width="8.53125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -809,33 +776,24 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="3">
         <v>43831</v>
@@ -844,27 +802,18 @@
         <v>2000000</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3">
         <v>44197</v>
@@ -873,27 +822,18 @@
         <v>2000000</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3">
         <v>44562</v>
@@ -902,30 +842,21 @@
         <v>1000000</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3">
         <v>43831</v>
@@ -934,16 +865,7 @@
         <v>2000000</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>